<commit_message>
Importing new substitute lists in a scheduled job running after app startup
</commit_message>
<xml_diff>
--- a/src/test/resources/substituttlister/test_substituttlister_sletting.xlsx
+++ b/src/test/resources/substituttlister/test_substituttlister_sletting.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aasmund/dev/hm-grunndata-alternativprodukter2/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aasmund/dev/hm-grunndata-alternativprodukter/src/test/resources/substituttlister/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39110B97-FEB7-F74E-AB77-4842E04B8EEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC0343F-8896-4845-B14B-45C6FCDEAD04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="16700" xr2:uid="{8997ABA3-265C-4565-AD00-094E7F16CC3A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Hms-nr</t>
   </si>
@@ -44,93 +44,12 @@
     <t>Overflyttingsplattform med sete</t>
   </si>
   <si>
-    <t>Sara Stedy</t>
-  </si>
-  <si>
-    <t>Sara Stedy, small</t>
-  </si>
-  <si>
     <t>Overflyttingsplattform uten sete</t>
   </si>
   <si>
-    <t>Etac Turner Pro</t>
-  </si>
-  <si>
     <t>Mobil personløfter for aktivt løft</t>
   </si>
   <si>
-    <t>ISA</t>
-  </si>
-  <si>
-    <t>Molift Quick Raiser</t>
-  </si>
-  <si>
-    <t>Sara Flex</t>
-  </si>
-  <si>
-    <t>162798</t>
-  </si>
-  <si>
-    <t>MiniLift</t>
-  </si>
-  <si>
-    <t>163388</t>
-  </si>
-  <si>
-    <t>023661</t>
-  </si>
-  <si>
-    <t>Nova 500 Mobil</t>
-  </si>
-  <si>
-    <t>162638</t>
-  </si>
-  <si>
-    <t>Nova 500NG Mobil Oppr.l</t>
-  </si>
-  <si>
-    <t>196087</t>
-  </si>
-  <si>
-    <t>Oxford Ascend</t>
-  </si>
-  <si>
-    <t>153174</t>
-  </si>
-  <si>
-    <t>161460</t>
-  </si>
-  <si>
-    <t>Oxford Journey</t>
-  </si>
-  <si>
-    <t>Sabina</t>
-  </si>
-  <si>
-    <t>021787</t>
-  </si>
-  <si>
-    <t>014760</t>
-  </si>
-  <si>
-    <t>149875</t>
-  </si>
-  <si>
-    <t>Sara 3000</t>
-  </si>
-  <si>
-    <t>Sara Plus</t>
-  </si>
-  <si>
-    <t>147286</t>
-  </si>
-  <si>
-    <t>ReTurn</t>
-  </si>
-  <si>
-    <t>113683</t>
-  </si>
-  <si>
     <t>Molift Raiser Pro</t>
   </si>
   <si>
@@ -153,9 +72,6 @@
   </si>
   <si>
     <t>Delkontraktbeskrivelse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GTP1 </t>
   </si>
   <si>
     <t>Kommentarer</t>
@@ -820,7 +736,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="C16" sqref="C16:D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -837,19 +753,19 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="F1" s="41"/>
       <c r="G1" s="47"/>
@@ -862,7 +778,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="12"/>
@@ -876,12 +792,8 @@
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="34"/>
       <c r="B3" s="20"/>
-      <c r="C3" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="12">
-        <v>232472</v>
-      </c>
+      <c r="C3" s="27"/>
+      <c r="D3" s="12"/>
       <c r="E3" s="8"/>
       <c r="F3" s="42"/>
       <c r="G3" s="47"/>
@@ -892,12 +804,8 @@
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="35"/>
       <c r="B4" s="21"/>
-      <c r="C4" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="13">
-        <v>292546</v>
-      </c>
+      <c r="C4" s="27"/>
+      <c r="D4" s="13"/>
       <c r="E4" s="6"/>
       <c r="F4" s="43"/>
       <c r="G4" s="48"/>
@@ -908,12 +816,8 @@
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="34"/>
       <c r="B5" s="20"/>
-      <c r="C5" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>30</v>
-      </c>
+      <c r="C5" s="27"/>
+      <c r="D5" s="13"/>
       <c r="E5" s="3"/>
       <c r="F5" s="6"/>
     </row>
@@ -929,45 +833,45 @@
       <c r="A7" s="34"/>
       <c r="B7" s="20"/>
       <c r="C7" s="28" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="7"/>
       <c r="G7" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="34"/>
       <c r="B8" s="20"/>
       <c r="C8" s="28" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="7"/>
       <c r="G8" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="34"/>
       <c r="B9" s="20"/>
       <c r="C9" s="28" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="7"/>
       <c r="G9" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -993,29 +897,18 @@
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="36"/>
       <c r="B12" s="22"/>
-      <c r="C12" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="14">
-        <v>184477</v>
-      </c>
+      <c r="C12" s="29"/>
+      <c r="D12" s="14"/>
       <c r="E12" s="4"/>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="36"/>
       <c r="B13" s="22"/>
-      <c r="C13" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="14">
-        <v>292535</v>
-      </c>
+      <c r="C13" s="29"/>
+      <c r="D13" s="14"/>
       <c r="E13" s="4"/>
       <c r="F13" s="2"/>
-      <c r="G13" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="36"/>
@@ -1030,7 +923,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C15" s="30"/>
       <c r="D15" s="15"/>
@@ -1040,36 +933,24 @@
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="37"/>
       <c r="B16" s="23"/>
-      <c r="C16" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="15">
-        <v>292483</v>
-      </c>
+      <c r="C16" s="30"/>
+      <c r="D16" s="15"/>
       <c r="E16" s="9"/>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="37"/>
       <c r="B17" s="23"/>
-      <c r="C17" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="16">
-        <v>242529</v>
-      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="16"/>
       <c r="E17" s="9"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="38"/>
       <c r="B18" s="24"/>
-      <c r="C18" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="15">
-        <v>242660</v>
-      </c>
+      <c r="C18" s="31"/>
+      <c r="D18" s="15"/>
       <c r="E18" s="5"/>
       <c r="F18" s="2"/>
     </row>
@@ -1081,51 +962,35 @@
       <c r="E19" s="5"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="37"/>
       <c r="B20" s="23"/>
-      <c r="C20" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>10</v>
-      </c>
+      <c r="C20" s="31"/>
+      <c r="D20" s="15"/>
       <c r="E20" s="5"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="37"/>
       <c r="B21" s="23"/>
-      <c r="C21" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>12</v>
-      </c>
+      <c r="C21" s="31"/>
+      <c r="D21" s="15"/>
       <c r="E21" s="5"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="37"/>
       <c r="B22" s="23"/>
-      <c r="C22" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>13</v>
-      </c>
+      <c r="C22" s="31"/>
+      <c r="D22" s="15"/>
       <c r="E22" s="5"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="37"/>
       <c r="B23" s="23"/>
-      <c r="C23" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>15</v>
-      </c>
+      <c r="C23" s="31"/>
+      <c r="D23" s="15"/>
       <c r="E23" s="5"/>
       <c r="F23" s="2"/>
     </row>
@@ -1137,87 +1002,59 @@
       <c r="E24" s="5"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="37"/>
       <c r="B25" s="23"/>
-      <c r="C25" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>17</v>
-      </c>
+      <c r="C25" s="31"/>
+      <c r="D25" s="15"/>
       <c r="E25" s="5"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="37"/>
       <c r="B26" s="23"/>
-      <c r="C26" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>19</v>
-      </c>
+      <c r="C26" s="31"/>
+      <c r="D26" s="15"/>
       <c r="E26" s="5"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="37"/>
       <c r="B27" s="23"/>
-      <c r="C27" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>20</v>
-      </c>
+      <c r="C27" s="31"/>
+      <c r="D27" s="15"/>
       <c r="E27" s="5"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="37"/>
       <c r="B28" s="23"/>
-      <c r="C28" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>23</v>
-      </c>
+      <c r="C28" s="31"/>
+      <c r="D28" s="15"/>
       <c r="E28" s="5"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="37"/>
       <c r="B29" s="23"/>
-      <c r="C29" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>24</v>
-      </c>
+      <c r="C29" s="31"/>
+      <c r="D29" s="15"/>
       <c r="E29" s="5"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="37"/>
       <c r="B30" s="23"/>
-      <c r="C30" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>25</v>
-      </c>
+      <c r="C30" s="31"/>
+      <c r="D30" s="15"/>
       <c r="E30" s="5"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="37"/>
       <c r="B31" s="23"/>
-      <c r="C31" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="C31" s="31"/>
+      <c r="D31" s="15"/>
       <c r="E31" s="5"/>
       <c r="F31" s="2"/>
     </row>

</xml_diff>